<commit_message>
updated excel file, include link to plotly
</commit_message>
<xml_diff>
--- a/RunOrWalk/AccuracyVStimeVSsamplesize.xlsx
+++ b/RunOrWalk/AccuracyVStimeVSsamplesize.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>Accuracy</t>
   </si>
@@ -57,18 +57,27 @@
   <si>
     <t>no.Windows</t>
   </si>
+  <si>
+    <t>https://plot.ly/~e0032186/1/#plot</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -91,8 +100,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -923,9 +933,15 @@
         <v>1.6540999999999999</v>
       </c>
     </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C22" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>